<commit_message>
map literature to taxonomy and create a matrix of local/global with specific and agnostic
</commit_message>
<xml_diff>
--- a/literature-mapping.xlsx
+++ b/literature-mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joa24jm\Documents\literature_review\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2ED8767-E57B-48BB-A96A-7D9EF98E891A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2383EB30-BA31-43B8-8747-56C4D6536081}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-8445" windowWidth="16440" windowHeight="28440" xr2:uid="{761C0854-549B-4FFA-AB58-89035C633947}"/>
+    <workbookView xWindow="-15220" yWindow="-14510" windowWidth="51420" windowHeight="14020" xr2:uid="{761C0854-549B-4FFA-AB58-89035C633947}"/>
   </bookViews>
   <sheets>
     <sheet name="method-taxonomy" sheetId="1" r:id="rId1"/>
@@ -33,8 +33,76 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={61826EBC-C90D-46E0-A52C-EDAD5A91D669}</author>
+    <author>tc={C120ED89-F58E-4D15-B0E5-7F6946C6A409}</author>
+    <author>tc={A29DE0E8-F745-42B3-BECC-FB7A240B5062}</author>
+    <author>tc={2FF89E20-286C-4992-A861-6FBCE8910FB6}</author>
+    <author>tc={E272C3E7-7777-4FC2-8167-376B2AE8EEA4}</author>
+    <author>tc={0EDFCB23-2BED-461A-8565-07DC8D3CBAAF}</author>
+  </authors>
+  <commentList>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{61826EBC-C90D-46E0-A52C-EDAD5A91D669}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Model-specific interpretation tools are limited to specific model classes. The interpretation of regression weights in a linear model is a model-specific interpretation, since – by definition – the interpretation of intrinsically interpretable models is always model-specific. Tools that only work for the interpretation of e.g. neural networks are model-specific</t>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="1" shapeId="0" xr:uid="{C120ED89-F58E-4D15-B0E5-7F6946C6A409}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Model-agnostic tools can be used on any machine learning model and are applied after the model has been trained (post hoc). These agnostic methods usually work by analyzing feature input and output pairs. By definition, these methods cannot have access to model internals such as weights or structural information</t>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="2" shapeId="0" xr:uid="{A29DE0E8-F745-42B3-BECC-FB7A240B5062}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    the interpretation method explains an individual prediction</t>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="3" shapeId="0" xr:uid="{2FF89E20-286C-4992-A861-6FBCE8910FB6}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    The interpretation method explains the entire model behavior.</t>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="4" shapeId="0" xr:uid="{E272C3E7-7777-4FC2-8167-376B2AE8EEA4}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Intrinsic interpretability can be achieved by designing self-
+explanatory models which incorporate interpretability di-
+rectly into the model structures.</t>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="5" shapeId="0" xr:uid="{0EDFCB23-2BED-461A-8565-07DC8D3CBAAF}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Post-hoc global explanation aims to provide a global un-
+derstanding about what knowledge has been acquired by
+these pre-trained models, and illuminate the parameters or
+learned representations in an intuitive manner to humans.</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>Model Specific</t>
   </si>
@@ -103,13 +171,16 @@
   </si>
   <si>
     <t>Individual Conditional Expectation</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -129,6 +200,12 @@
       <name val="CMU Serif"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -138,7 +215,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -147,29 +224,15 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
+      <left style="thin">
         <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
+      <top style="thin">
         <color indexed="64"/>
-      </right>
-      <top/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -183,14 +246,27 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -201,6 +277,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Johannes Allgaier" id="{177DFE44-CC35-4760-A64B-8C2F670CCC4A}" userId="Johannes Allgaier" providerId="None"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -498,31 +580,58 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="B1" dT="2021-11-16T13:20:05.50" personId="{177DFE44-CC35-4760-A64B-8C2F670CCC4A}" id="{61826EBC-C90D-46E0-A52C-EDAD5A91D669}">
+    <text>Model-specific interpretation tools are limited to specific model classes. The interpretation of regression weights in a linear model is a model-specific interpretation, since – by definition – the interpretation of intrinsically interpretable models is always model-specific. Tools that only work for the interpretation of e.g. neural networks are model-specific</text>
+  </threadedComment>
+  <threadedComment ref="C1" dT="2021-11-16T13:20:46.10" personId="{177DFE44-CC35-4760-A64B-8C2F670CCC4A}" id="{C120ED89-F58E-4D15-B0E5-7F6946C6A409}">
+    <text>Model-agnostic tools can be used on any machine learning model and are applied after the model has been trained (post hoc). These agnostic methods usually work by analyzing feature input and output pairs. By definition, these methods cannot have access to model internals such as weights or structural information</text>
+  </threadedComment>
+  <threadedComment ref="D1" dT="2021-11-16T13:21:18.37" personId="{177DFE44-CC35-4760-A64B-8C2F670CCC4A}" id="{A29DE0E8-F745-42B3-BECC-FB7A240B5062}">
+    <text>the interpretation method explains an individual prediction</text>
+  </threadedComment>
+  <threadedComment ref="E1" dT="2021-11-16T13:21:43.91" personId="{177DFE44-CC35-4760-A64B-8C2F670CCC4A}" id="{2FF89E20-286C-4992-A861-6FBCE8910FB6}">
+    <text>The interpretation method explains the entire model behavior.</text>
+  </threadedComment>
+  <threadedComment ref="F1" dT="2021-11-16T13:27:58.57" personId="{177DFE44-CC35-4760-A64B-8C2F670CCC4A}" id="{E272C3E7-7777-4FC2-8167-376B2AE8EEA4}">
+    <text>Intrinsic interpretability can be achieved by designing self-
+explanatory models which incorporate interpretability di-
+rectly into the model structures.</text>
+  </threadedComment>
+  <threadedComment ref="G1" dT="2021-11-16T13:32:35.62" personId="{177DFE44-CC35-4760-A64B-8C2F670CCC4A}" id="{0EDFCB23-2BED-461A-8565-07DC8D3CBAAF}">
+    <text>Post-hoc global explanation aims to provide a global un-
+derstanding about what knowledge has been acquired by
+these pre-trained models, and illuminate the parameters or
+learned representations in an intuitive manner to humans.</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAC18D3B-4635-4B61-AF0F-2FFBD05B0AA5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAC18D3B-4635-4B61-AF0F-2FFBD05B0AA5}">
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="34.69921875" customWidth="1"/>
-    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.09765625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.59765625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.09765625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.59765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="9.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="29.3984375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="21.09765625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="21.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="16.2" x14ac:dyDescent="0.4">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -545,89 +654,194 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="B2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A17" s="3" t="s">
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G16">
     <sortCondition ref="A2:A16"/>
   </sortState>
+  <conditionalFormatting sqref="B2:G17">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"x"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{9297248C-A4EF-4C8C-8377-51CEE826DE6B}"/>
     <hyperlink ref="A3" r:id="rId2" xr:uid="{35EF1A83-75D2-4EA9-A395-17A39E0DAEA5}"/>
@@ -648,5 +862,6 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId17"/>
+  <legacyDrawing r:id="rId18"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Check Google's Explainable AI Whitepaper
Get content from the paper adapted to the own paper.
</commit_message>
<xml_diff>
--- a/literature-mapping.xlsx
+++ b/literature-mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joa24jm\Documents\literature_review\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2383EB30-BA31-43B8-8747-56C4D6536081}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DEB2C8A-AE0B-48A4-BA69-856C0BE12BAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15220" yWindow="-14510" windowWidth="51420" windowHeight="14020" xr2:uid="{761C0854-549B-4FFA-AB58-89035C633947}"/>
+    <workbookView xWindow="2388" yWindow="0" windowWidth="17208" windowHeight="10296" xr2:uid="{761C0854-549B-4FFA-AB58-89035C633947}"/>
   </bookViews>
   <sheets>
     <sheet name="method-taxonomy" sheetId="1" r:id="rId1"/>
@@ -42,6 +42,10 @@
     <author>tc={2FF89E20-286C-4992-A861-6FBCE8910FB6}</author>
     <author>tc={E272C3E7-7777-4FC2-8167-376B2AE8EEA4}</author>
     <author>tc={0EDFCB23-2BED-461A-8565-07DC8D3CBAAF}</author>
+    <author>tc={78EFFE56-1FB0-40A8-B77A-512D48359E08}</author>
+    <author>tc={81562FEA-FE10-420A-B179-AE77E44CC4B1}</author>
+    <author>tc={D6875841-972F-4B52-8EA0-CFFFD8B4D214}</author>
+    <author>tc={2E75B4AD-9F22-44DB-9F89-A8147DDCCA6F}</author>
   </authors>
   <commentList>
     <comment ref="B1" authorId="0" shapeId="0" xr:uid="{61826EBC-C90D-46E0-A52C-EDAD5A91D669}">
@@ -97,12 +101,44 @@
 learned representations in an intuitive manner to humans.</t>
       </text>
     </comment>
+    <comment ref="A5" authorId="6" shapeId="0" xr:uid="{78EFFE56-1FB0-40A8-B77A-512D48359E08}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    In the familiy of gradient-based methods</t>
+      </text>
+    </comment>
+    <comment ref="A28" authorId="7" shapeId="0" xr:uid="{81562FEA-FE10-420A-B179-AE77E44CC4B1}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Recommended for tabular and non-differentiable models</t>
+      </text>
+    </comment>
+    <comment ref="A29" authorId="8" shapeId="0" xr:uid="{D6875841-972F-4B52-8EA0-CFFFD8B4D214}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    In the familiy of gradient-based methods</t>
+      </text>
+    </comment>
+    <comment ref="A30" authorId="9" shapeId="0" xr:uid="{2E75B4AD-9F22-44DB-9F89-A8147DDCCA6F}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    In the familiy of gradient-based methods</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="40">
   <si>
     <t>Model Specific</t>
   </si>
@@ -125,9 +161,6 @@
     <t>Permutation Importance</t>
   </si>
   <si>
-    <t>SHAP</t>
-  </si>
-  <si>
     <t>LIME</t>
   </si>
   <si>
@@ -152,9 +185,6 @@
     <t>TabNet</t>
   </si>
   <si>
-    <t>TensorFlow Lattice</t>
-  </si>
-  <si>
     <t>Partial Dependence Plots</t>
   </si>
   <si>
@@ -173,14 +203,130 @@
     <t>Individual Conditional Expectation</t>
   </si>
   <si>
-    <t>x</t>
+    <t>Anchors</t>
+  </si>
+  <si>
+    <t>LOCO</t>
+  </si>
+  <si>
+    <t>XRAI</t>
+  </si>
+  <si>
+    <t>DeepR</t>
+  </si>
+  <si>
+    <t>Automatic Concept-based Explanations</t>
+  </si>
+  <si>
+    <t>MMD Critic</t>
+  </si>
+  <si>
+    <t>Representer Point Selection</t>
+  </si>
+  <si>
+    <t>Influence Functions</t>
+  </si>
+  <si>
+    <t>Attention Based Protocol Learning</t>
+  </si>
+  <si>
+    <t>NN to Decistion Tree</t>
+  </si>
+  <si>
+    <t>Deep Lattice Networks 
+and Partial Monotonic Functions</t>
+  </si>
+  <si>
+    <t>Adresses
+Computer Vision Tasks</t>
+  </si>
+  <si>
+    <t>Adresses
+Neural Networks</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>Sampling Shapley</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="10"/>
+        <rFont val="CMU Serif"/>
+      </rPr>
+      <t>SH</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="10"/>
+        <rFont val="CMU Serif"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">apely </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="10"/>
+        <rFont val="CMU Serif"/>
+      </rPr>
+      <t>A</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="10"/>
+        <rFont val="CMU Serif"/>
+        <family val="2"/>
+      </rPr>
+      <t>dditive ex</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="10"/>
+        <rFont val="CMU Serif"/>
+      </rPr>
+      <t>P</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="10"/>
+        <rFont val="CMU Serif"/>
+        <family val="2"/>
+      </rPr>
+      <t>lanations</t>
+    </r>
+  </si>
+  <si>
+    <t>Grad-CAM</t>
+  </si>
+  <si>
+    <t>SmoothGrad</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -205,6 +351,25 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="CMU Serif"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="CMU Serif"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -243,19 +408,144 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -605,241 +895,515 @@
 these pre-trained models, and illuminate the parameters or
 learned representations in an intuitive manner to humans.</text>
   </threadedComment>
+  <threadedComment ref="A5" dT="2021-11-18T11:25:27.19" personId="{177DFE44-CC35-4760-A64B-8C2F670CCC4A}" id="{78EFFE56-1FB0-40A8-B77A-512D48359E08}">
+    <text>In the familiy of gradient-based methods</text>
+  </threadedComment>
+  <threadedComment ref="A28" dT="2021-11-18T11:20:26.94" personId="{177DFE44-CC35-4760-A64B-8C2F670CCC4A}" id="{81562FEA-FE10-420A-B179-AE77E44CC4B1}">
+    <text>Recommended for tabular and non-differentiable models</text>
+  </threadedComment>
+  <threadedComment ref="A29" dT="2021-11-18T11:24:28.90" personId="{177DFE44-CC35-4760-A64B-8C2F670CCC4A}" id="{D6875841-972F-4B52-8EA0-CFFFD8B4D214}">
+    <text>In the familiy of gradient-based methods</text>
+  </threadedComment>
+  <threadedComment ref="A30" dT="2021-11-18T11:24:34.40" personId="{177DFE44-CC35-4760-A64B-8C2F670CCC4A}" id="{2E75B4AD-9F22-44DB-9F89-A8147DDCCA6F}">
+    <text>In the familiy of gradient-based methods</text>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAC18D3B-4635-4B61-AF0F-2FFBD05B0AA5}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.69921875" customWidth="1"/>
+    <col min="1" max="1" width="34.19921875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.59765625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.796875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.59765625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="29.3984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.8984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.3984375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="21.09765625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="21.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16.2" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9" ht="31.2" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="2"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="2"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="2"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="2"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="2"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="2"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="2"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="2"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="2"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="2"/>
+    </row>
+    <row r="14" spans="1:9" ht="31.2" x14ac:dyDescent="0.35">
+      <c r="A14" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="2"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A15" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="2"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A16" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="2"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A17" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="2"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A18" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="3" t="s">
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="2"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A19" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="2"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A20" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
+      <c r="B20" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A21" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="2"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A22" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="2"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A23" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="2"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A24" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="2"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A25" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="2"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A26" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="2"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A27" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="2"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A28" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A29" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A30" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G16">
     <sortCondition ref="A2:A16"/>
   </sortState>
   <conditionalFormatting sqref="B2:G17">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
       <formula>"x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B20">
+    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
+      <formula>"x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D20">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
+      <formula>"x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:XFD1048576">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+      <formula>"yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"no"</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
@@ -853,15 +1417,28 @@
     <hyperlink ref="A8" r:id="rId8" location="metadata_info_tab_contents" xr:uid="{2E433A07-C6E1-4958-8C95-4D8FE54A710E}"/>
     <hyperlink ref="A9" r:id="rId9" xr:uid="{2DC32FDB-531D-4E42-8D95-1F6298EA7F48}"/>
     <hyperlink ref="A10" r:id="rId10" xr:uid="{1C176282-DED7-4CFE-834C-DD7EFA12E1B9}"/>
-    <hyperlink ref="A11" r:id="rId11" xr:uid="{27F60B6A-AD95-4A31-B7BB-A255EBB1B59B}"/>
+    <hyperlink ref="A11" r:id="rId11" display="SHAP" xr:uid="{27F60B6A-AD95-4A31-B7BB-A255EBB1B59B}"/>
     <hyperlink ref="A12" r:id="rId12" xr:uid="{90885111-5403-4CF9-BC57-3C31EF0AE4A3}"/>
     <hyperlink ref="A13" r:id="rId13" xr:uid="{D1701D65-C3E9-44B9-9432-6DE16CD43459}"/>
-    <hyperlink ref="A14" r:id="rId14" xr:uid="{C40B8795-0355-46FD-85E9-F08955370F28}"/>
+    <hyperlink ref="A14" r:id="rId14" display="Deep Lattice Networks and Partial Monotonic Functions" xr:uid="{C40B8795-0355-46FD-85E9-F08955370F28}"/>
     <hyperlink ref="A16" r:id="rId15" xr:uid="{958B5310-3407-4F42-BF4D-D61F37FFA816}"/>
     <hyperlink ref="A17" r:id="rId16" xr:uid="{09E41EEB-2EC0-4EB6-88B7-8F6E25E15238}"/>
+    <hyperlink ref="A18" r:id="rId17" xr:uid="{72E3E7BC-7B2E-4618-A58A-149793960C7F}"/>
+    <hyperlink ref="A19" r:id="rId18" xr:uid="{20B83A96-428E-4479-A9D3-636F03504E2C}"/>
+    <hyperlink ref="A20" r:id="rId19" xr:uid="{D05401CB-7A16-46FE-82D1-13E9C9B73EBE}"/>
+    <hyperlink ref="A21" r:id="rId20" xr:uid="{9FD4428F-7748-4B69-9C49-BCD0EBA035C9}"/>
+    <hyperlink ref="A22" r:id="rId21" xr:uid="{FBDDE59E-EEC1-439C-A1C0-552D68A350ED}"/>
+    <hyperlink ref="A23" r:id="rId22" xr:uid="{DC3C4241-0BCD-4AA5-9599-E5C0FD1B0A67}"/>
+    <hyperlink ref="A24" r:id="rId23" xr:uid="{C50A4BC1-DC3A-4E06-AE5F-1FDA87C12F5E}"/>
+    <hyperlink ref="A25" r:id="rId24" xr:uid="{2F0F98AE-1E27-4C0D-9C25-E88E96D09296}"/>
+    <hyperlink ref="A26" r:id="rId25" xr:uid="{8FD0B6DE-815B-4968-BF82-F3A750F3FF0A}"/>
+    <hyperlink ref="A27" r:id="rId26" xr:uid="{4F8113ED-4F92-4A42-9BF6-8AE87E627AED}"/>
+    <hyperlink ref="A28" r:id="rId27" xr:uid="{042875D8-C34B-4E02-BDED-CE45E506DF4A}"/>
+    <hyperlink ref="A29" r:id="rId28" xr:uid="{02F2BFA7-7428-4B13-9C17-18BF77735185}"/>
+    <hyperlink ref="A30" r:id="rId29" xr:uid="{0B060E60-6089-4CFC-875F-4F2F9213E464}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId17"/>
-  <legacyDrawing r:id="rId18"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId30"/>
+  <legacyDrawing r:id="rId31"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add some explainability papers and update excel
Add source code availability column
</commit_message>
<xml_diff>
--- a/literature-mapping.xlsx
+++ b/literature-mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joa24jm\Documents\literature_review\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DEB2C8A-AE0B-48A4-BA69-856C0BE12BAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5CF0D90-D7E1-4654-9FCB-013B4B81B650}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2388" yWindow="0" windowWidth="17208" windowHeight="10296" xr2:uid="{761C0854-549B-4FFA-AB58-89035C633947}"/>
+    <workbookView xWindow="-8130" yWindow="-12550" windowWidth="38400" windowHeight="10100" xr2:uid="{761C0854-549B-4FFA-AB58-89035C633947}"/>
   </bookViews>
   <sheets>
     <sheet name="method-taxonomy" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
     <author>tc={2E75B4AD-9F22-44DB-9F89-A8147DDCCA6F}</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{61826EBC-C90D-46E0-A52C-EDAD5A91D669}">
+    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{61826EBC-C90D-46E0-A52C-EDAD5A91D669}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -56,7 +56,7 @@
     Model-specific interpretation tools are limited to specific model classes. The interpretation of regression weights in a linear model is a model-specific interpretation, since – by definition – the interpretation of intrinsically interpretable models is always model-specific. Tools that only work for the interpretation of e.g. neural networks are model-specific</t>
       </text>
     </comment>
-    <comment ref="C1" authorId="1" shapeId="0" xr:uid="{C120ED89-F58E-4D15-B0E5-7F6946C6A409}">
+    <comment ref="C2" authorId="1" shapeId="0" xr:uid="{C120ED89-F58E-4D15-B0E5-7F6946C6A409}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -64,7 +64,7 @@
     Model-agnostic tools can be used on any machine learning model and are applied after the model has been trained (post hoc). These agnostic methods usually work by analyzing feature input and output pairs. By definition, these methods cannot have access to model internals such as weights or structural information</t>
       </text>
     </comment>
-    <comment ref="D1" authorId="2" shapeId="0" xr:uid="{A29DE0E8-F745-42B3-BECC-FB7A240B5062}">
+    <comment ref="D2" authorId="2" shapeId="0" xr:uid="{A29DE0E8-F745-42B3-BECC-FB7A240B5062}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -72,7 +72,7 @@
     the interpretation method explains an individual prediction</t>
       </text>
     </comment>
-    <comment ref="E1" authorId="3" shapeId="0" xr:uid="{2FF89E20-286C-4992-A861-6FBCE8910FB6}">
+    <comment ref="E2" authorId="3" shapeId="0" xr:uid="{2FF89E20-286C-4992-A861-6FBCE8910FB6}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -80,7 +80,7 @@
     The interpretation method explains the entire model behavior.</t>
       </text>
     </comment>
-    <comment ref="F1" authorId="4" shapeId="0" xr:uid="{E272C3E7-7777-4FC2-8167-376B2AE8EEA4}">
+    <comment ref="F2" authorId="4" shapeId="0" xr:uid="{E272C3E7-7777-4FC2-8167-376B2AE8EEA4}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -90,7 +90,7 @@
 rectly into the model structures.</t>
       </text>
     </comment>
-    <comment ref="G1" authorId="5" shapeId="0" xr:uid="{0EDFCB23-2BED-461A-8565-07DC8D3CBAAF}">
+    <comment ref="G2" authorId="5" shapeId="0" xr:uid="{0EDFCB23-2BED-461A-8565-07DC8D3CBAAF}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -98,10 +98,14 @@
     Post-hoc global explanation aims to provide a global un-
 derstanding about what knowledge has been acquired by
 these pre-trained models, and illuminate the parameters or
-learned representations in an intuitive manner to humans.</t>
+learned representations in an intuitive manner to humans.
+Reply:
+    Post-hoc XAI methods approximate the behavior of a black-box by extracting relationships between feature values and the predictions. https://www.sciencedirect.com/science/article/pii/S0957417420307302
+Reply:
+    and post-hoc explainability - methods that analyse the model after training. Post-hoc techniques refer to the global and local techniques described earlier. - Rhys Ward</t>
       </text>
     </comment>
-    <comment ref="A5" authorId="6" shapeId="0" xr:uid="{78EFFE56-1FB0-40A8-B77A-512D48359E08}">
+    <comment ref="A6" authorId="6" shapeId="0" xr:uid="{78EFFE56-1FB0-40A8-B77A-512D48359E08}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -138,7 +142,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="44">
   <si>
     <t>Model Specific</t>
   </si>
@@ -165,12 +169,6 @@
   </si>
   <si>
     <t>Q-FIT</t>
-  </si>
-  <si>
-    <t>S-LIME</t>
-  </si>
-  <si>
-    <t>DeepLIFT</t>
   </si>
   <si>
     <t>Layer-Wise Relevane Propagation</t>
@@ -321,12 +319,30 @@
   <si>
     <t>SmoothGrad</t>
   </si>
+  <si>
+    <t>DeepLIFT (Deep Learning Important FeaTures)</t>
+  </si>
+  <si>
+    <t>Year of publication</t>
+  </si>
+  <si>
+    <t>Explainable Tasks</t>
+  </si>
+  <si>
+    <t>Classification</t>
+  </si>
+  <si>
+    <t>Regression, Classification</t>
+  </si>
+  <si>
+    <t>Source Code Available</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -347,12 +363,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <b/>
       <u/>
       <sz val="11"/>
@@ -364,12 +374,6 @@
       <sz val="11"/>
       <color theme="10"/>
       <name val="CMU Serif"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -408,7 +412,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -427,15 +431,22 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="5">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -486,76 +497,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -567,6 +508,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>11955</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>119199</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>606583</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>156750</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B62CEB96-5029-4AE6-9D42-20084F743918}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16521955" y="119199"/>
+          <a:ext cx="7977501" cy="6406964"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
@@ -872,30 +862,36 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="B1" dT="2021-11-16T13:20:05.50" personId="{177DFE44-CC35-4760-A64B-8C2F670CCC4A}" id="{61826EBC-C90D-46E0-A52C-EDAD5A91D669}">
+  <threadedComment ref="B2" dT="2021-11-16T13:20:05.50" personId="{177DFE44-CC35-4760-A64B-8C2F670CCC4A}" id="{61826EBC-C90D-46E0-A52C-EDAD5A91D669}">
     <text>Model-specific interpretation tools are limited to specific model classes. The interpretation of regression weights in a linear model is a model-specific interpretation, since – by definition – the interpretation of intrinsically interpretable models is always model-specific. Tools that only work for the interpretation of e.g. neural networks are model-specific</text>
   </threadedComment>
-  <threadedComment ref="C1" dT="2021-11-16T13:20:46.10" personId="{177DFE44-CC35-4760-A64B-8C2F670CCC4A}" id="{C120ED89-F58E-4D15-B0E5-7F6946C6A409}">
+  <threadedComment ref="C2" dT="2021-11-16T13:20:46.10" personId="{177DFE44-CC35-4760-A64B-8C2F670CCC4A}" id="{C120ED89-F58E-4D15-B0E5-7F6946C6A409}">
     <text>Model-agnostic tools can be used on any machine learning model and are applied after the model has been trained (post hoc). These agnostic methods usually work by analyzing feature input and output pairs. By definition, these methods cannot have access to model internals such as weights or structural information</text>
   </threadedComment>
-  <threadedComment ref="D1" dT="2021-11-16T13:21:18.37" personId="{177DFE44-CC35-4760-A64B-8C2F670CCC4A}" id="{A29DE0E8-F745-42B3-BECC-FB7A240B5062}">
+  <threadedComment ref="D2" dT="2021-11-16T13:21:18.37" personId="{177DFE44-CC35-4760-A64B-8C2F670CCC4A}" id="{A29DE0E8-F745-42B3-BECC-FB7A240B5062}">
     <text>the interpretation method explains an individual prediction</text>
   </threadedComment>
-  <threadedComment ref="E1" dT="2021-11-16T13:21:43.91" personId="{177DFE44-CC35-4760-A64B-8C2F670CCC4A}" id="{2FF89E20-286C-4992-A861-6FBCE8910FB6}">
+  <threadedComment ref="E2" dT="2021-11-16T13:21:43.91" personId="{177DFE44-CC35-4760-A64B-8C2F670CCC4A}" id="{2FF89E20-286C-4992-A861-6FBCE8910FB6}">
     <text>The interpretation method explains the entire model behavior.</text>
   </threadedComment>
-  <threadedComment ref="F1" dT="2021-11-16T13:27:58.57" personId="{177DFE44-CC35-4760-A64B-8C2F670CCC4A}" id="{E272C3E7-7777-4FC2-8167-376B2AE8EEA4}">
+  <threadedComment ref="F2" dT="2021-11-16T13:27:58.57" personId="{177DFE44-CC35-4760-A64B-8C2F670CCC4A}" id="{E272C3E7-7777-4FC2-8167-376B2AE8EEA4}">
     <text>Intrinsic interpretability can be achieved by designing self-
 explanatory models which incorporate interpretability di-
 rectly into the model structures.</text>
   </threadedComment>
-  <threadedComment ref="G1" dT="2021-11-16T13:32:35.62" personId="{177DFE44-CC35-4760-A64B-8C2F670CCC4A}" id="{0EDFCB23-2BED-461A-8565-07DC8D3CBAAF}">
+  <threadedComment ref="G2" dT="2021-11-16T13:32:35.62" personId="{177DFE44-CC35-4760-A64B-8C2F670CCC4A}" id="{0EDFCB23-2BED-461A-8565-07DC8D3CBAAF}">
     <text>Post-hoc global explanation aims to provide a global un-
 derstanding about what knowledge has been acquired by
 these pre-trained models, and illuminate the parameters or
 learned representations in an intuitive manner to humans.</text>
   </threadedComment>
-  <threadedComment ref="A5" dT="2021-11-18T11:25:27.19" personId="{177DFE44-CC35-4760-A64B-8C2F670CCC4A}" id="{78EFFE56-1FB0-40A8-B77A-512D48359E08}">
+  <threadedComment ref="G2" dT="2021-11-19T09:35:12.63" personId="{177DFE44-CC35-4760-A64B-8C2F670CCC4A}" id="{885BDCFE-EEBE-4C40-96D0-8EA9932D96F9}" parentId="{0EDFCB23-2BED-461A-8565-07DC8D3CBAAF}">
+    <text>Post-hoc XAI methods approximate the behavior of a black-box by extracting relationships between feature values and the predictions. https://www.sciencedirect.com/science/article/pii/S0957417420307302</text>
+  </threadedComment>
+  <threadedComment ref="G2" dT="2021-11-19T14:22:18.64" personId="{177DFE44-CC35-4760-A64B-8C2F670CCC4A}" id="{8E9CB568-009E-4068-9EDB-77FEBEA42AE1}" parentId="{0EDFCB23-2BED-461A-8565-07DC8D3CBAAF}">
+    <text>and post-hoc explainability - methods that analyse the model after training. Post-hoc techniques refer to the global and local techniques described earlier. - Rhys Ward</text>
+  </threadedComment>
+  <threadedComment ref="A6" dT="2021-11-18T11:25:27.19" personId="{177DFE44-CC35-4760-A64B-8C2F670CCC4A}" id="{78EFFE56-1FB0-40A8-B77A-512D48359E08}">
     <text>In the familiy of gradient-based methods</text>
   </threadedComment>
   <threadedComment ref="A28" dT="2021-11-18T11:20:26.94" personId="{177DFE44-CC35-4760-A64B-8C2F670CCC4A}" id="{81562FEA-FE10-420A-B179-AE77E44CC4B1}">
@@ -912,15 +908,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAC18D3B-4635-4B61-AF0F-2FFBD05B0AA5}">
-  <dimension ref="A1:I30"/>
+  <dimension ref="A2:L30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.19921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.3984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.59765625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.796875" bestFit="1" customWidth="1"/>
@@ -929,248 +925,528 @@
     <col min="7" max="7" width="9.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.8984375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23.3984375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.09765625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.59765625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19" customWidth="1"/>
+    <col min="11" max="11" width="23.3984375" customWidth="1"/>
+    <col min="12" max="12" width="22.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="31.2" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B1" s="3" t="s">
+    <row r="2" spans="1:12" ht="31.2" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" s="4" t="s">
+      <c r="H2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" s="2">
+        <v>2016</v>
+      </c>
+      <c r="K3" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="L3" s="2"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J4" s="2">
+        <v>2019</v>
+      </c>
+      <c r="K4" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="L4" s="2"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J5" s="2">
+        <v>2017</v>
+      </c>
+      <c r="K5" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="L5" s="2"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J6" s="11">
+        <v>2016</v>
+      </c>
+      <c r="K6" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="L6" s="2"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J7" s="11">
+        <v>2017</v>
+      </c>
+      <c r="K7" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="L7" s="2"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="5" t="s">
+      <c r="B8" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J8" s="11">
+        <v>2013</v>
+      </c>
+      <c r="K8" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="L8" s="2"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J9" s="2">
+        <v>2001</v>
+      </c>
+      <c r="K9" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="L9" s="2"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A10" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J10" s="2">
+        <v>2010</v>
+      </c>
+      <c r="K10" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="L10" s="2"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A11" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J11" s="2">
+        <v>2020</v>
+      </c>
+      <c r="K11" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="L11" s="2"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A12" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="2"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="2"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" s="4" t="s">
+      <c r="B12" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J12" s="2">
+        <v>2017</v>
+      </c>
+      <c r="K12" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A13" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J13" s="2">
+        <v>2020</v>
+      </c>
+      <c r="K13" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="31.2" x14ac:dyDescent="0.35">
+      <c r="A14" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J14" s="2">
+        <v>2017</v>
+      </c>
+      <c r="K14" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A15" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J15" s="2">
+        <v>2018</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A16" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="2"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="2"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="2"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="2"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="2"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="2"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A11" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="2"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A13" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="2"/>
-    </row>
-    <row r="14" spans="1:9" ht="31.2" x14ac:dyDescent="0.35">
-      <c r="A14" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="2"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A15" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="2"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A16" s="4" t="s">
-        <v>13</v>
       </c>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -1180,10 +1456,13 @@
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
       <c r="I16" s="2"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -1193,10 +1472,13 @@
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
       <c r="I17" s="2"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -1206,10 +1488,13 @@
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
       <c r="I18" s="2"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -1219,35 +1504,47 @@
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
       <c r="I19" s="2"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
+        <v>33</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>32</v>
+      </c>
       <c r="H20" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+      <c r="J20" s="2">
+        <v>2019</v>
+      </c>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -1257,10 +1554,13 @@
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
       <c r="I21" s="2"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -1270,10 +1570,13 @@
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
       <c r="I22" s="2"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -1283,10 +1586,13 @@
       <c r="G23" s="5"/>
       <c r="H23" s="5"/>
       <c r="I23" s="2"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
@@ -1296,10 +1602,13 @@
       <c r="G24" s="5"/>
       <c r="H24" s="5"/>
       <c r="I24" s="2"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
@@ -1309,10 +1618,13 @@
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
       <c r="I25" s="2"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
@@ -1322,10 +1634,13 @@
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
       <c r="I26" s="2"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A27" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
@@ -1335,10 +1650,13 @@
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
       <c r="I27" s="2"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -1347,15 +1665,18 @@
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -1365,10 +1686,13 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -1378,67 +1702,71 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G16">
-    <sortCondition ref="A2:A16"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:G16">
+    <sortCondition ref="A3:A16"/>
   </sortState>
-  <conditionalFormatting sqref="B2:G17">
-    <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
+  <conditionalFormatting sqref="B3:G17">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20">
-    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D20">
-    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:XFD1048576">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"no"</formula>
+    </cfRule>
     <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
-      <formula>"no"</formula>
-    </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{9297248C-A4EF-4C8C-8377-51CEE826DE6B}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{35EF1A83-75D2-4EA9-A395-17A39E0DAEA5}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{E9A918AD-248E-40D1-8057-6403249E6FEA}"/>
-    <hyperlink ref="A5" r:id="rId4" xr:uid="{8C3159B2-E126-480C-AAAE-178706B298A3}"/>
-    <hyperlink ref="A6" r:id="rId5" xr:uid="{818ABA6C-CC95-471F-B0AB-0D0BE5E8D539}"/>
+    <hyperlink ref="A3" r:id="rId1" display="DeepLIFT" xr:uid="{9297248C-A4EF-4C8C-8377-51CEE826DE6B}"/>
+    <hyperlink ref="A4" r:id="rId2" xr:uid="{35EF1A83-75D2-4EA9-A395-17A39E0DAEA5}"/>
+    <hyperlink ref="A5" r:id="rId3" xr:uid="{E9A918AD-248E-40D1-8057-6403249E6FEA}"/>
+    <hyperlink ref="A6" r:id="rId4" xr:uid="{8C3159B2-E126-480C-AAAE-178706B298A3}"/>
+    <hyperlink ref="A7" r:id="rId5" xr:uid="{818ABA6C-CC95-471F-B0AB-0D0BE5E8D539}"/>
     <hyperlink ref="A15" r:id="rId6" xr:uid="{B9B0F060-F95B-488E-B127-7BDAECBF80EC}"/>
-    <hyperlink ref="A7" r:id="rId7" xr:uid="{84CB77FD-EC6B-4043-A1B6-31A9B5D0838B}"/>
-    <hyperlink ref="A8" r:id="rId8" location="metadata_info_tab_contents" xr:uid="{2E433A07-C6E1-4958-8C95-4D8FE54A710E}"/>
-    <hyperlink ref="A9" r:id="rId9" xr:uid="{2DC32FDB-531D-4E42-8D95-1F6298EA7F48}"/>
-    <hyperlink ref="A10" r:id="rId10" xr:uid="{1C176282-DED7-4CFE-834C-DD7EFA12E1B9}"/>
-    <hyperlink ref="A11" r:id="rId11" display="SHAP" xr:uid="{27F60B6A-AD95-4A31-B7BB-A255EBB1B59B}"/>
-    <hyperlink ref="A12" r:id="rId12" xr:uid="{90885111-5403-4CF9-BC57-3C31EF0AE4A3}"/>
-    <hyperlink ref="A13" r:id="rId13" xr:uid="{D1701D65-C3E9-44B9-9432-6DE16CD43459}"/>
-    <hyperlink ref="A14" r:id="rId14" display="Deep Lattice Networks and Partial Monotonic Functions" xr:uid="{C40B8795-0355-46FD-85E9-F08955370F28}"/>
-    <hyperlink ref="A16" r:id="rId15" xr:uid="{958B5310-3407-4F42-BF4D-D61F37FFA816}"/>
-    <hyperlink ref="A17" r:id="rId16" xr:uid="{09E41EEB-2EC0-4EB6-88B7-8F6E25E15238}"/>
-    <hyperlink ref="A18" r:id="rId17" xr:uid="{72E3E7BC-7B2E-4618-A58A-149793960C7F}"/>
-    <hyperlink ref="A19" r:id="rId18" xr:uid="{20B83A96-428E-4479-A9D3-636F03504E2C}"/>
-    <hyperlink ref="A20" r:id="rId19" xr:uid="{D05401CB-7A16-46FE-82D1-13E9C9B73EBE}"/>
-    <hyperlink ref="A21" r:id="rId20" xr:uid="{9FD4428F-7748-4B69-9C49-BCD0EBA035C9}"/>
-    <hyperlink ref="A22" r:id="rId21" xr:uid="{FBDDE59E-EEC1-439C-A1C0-552D68A350ED}"/>
-    <hyperlink ref="A23" r:id="rId22" xr:uid="{DC3C4241-0BCD-4AA5-9599-E5C0FD1B0A67}"/>
-    <hyperlink ref="A24" r:id="rId23" xr:uid="{C50A4BC1-DC3A-4E06-AE5F-1FDA87C12F5E}"/>
-    <hyperlink ref="A25" r:id="rId24" xr:uid="{2F0F98AE-1E27-4C0D-9C25-E88E96D09296}"/>
-    <hyperlink ref="A26" r:id="rId25" xr:uid="{8FD0B6DE-815B-4968-BF82-F3A750F3FF0A}"/>
-    <hyperlink ref="A27" r:id="rId26" xr:uid="{4F8113ED-4F92-4A42-9BF6-8AE87E627AED}"/>
-    <hyperlink ref="A28" r:id="rId27" xr:uid="{042875D8-C34B-4E02-BDED-CE45E506DF4A}"/>
-    <hyperlink ref="A29" r:id="rId28" xr:uid="{02F2BFA7-7428-4B13-9C17-18BF77735185}"/>
-    <hyperlink ref="A30" r:id="rId29" xr:uid="{0B060E60-6089-4CFC-875F-4F2F9213E464}"/>
+    <hyperlink ref="A8" r:id="rId7" xr:uid="{84CB77FD-EC6B-4043-A1B6-31A9B5D0838B}"/>
+    <hyperlink ref="A9" r:id="rId8" location="metadata_info_tab_contents" xr:uid="{2E433A07-C6E1-4958-8C95-4D8FE54A710E}"/>
+    <hyperlink ref="A10" r:id="rId9" xr:uid="{2DC32FDB-531D-4E42-8D95-1F6298EA7F48}"/>
+    <hyperlink ref="A11" r:id="rId10" xr:uid="{1C176282-DED7-4CFE-834C-DD7EFA12E1B9}"/>
+    <hyperlink ref="A12" r:id="rId11" display="SHAP" xr:uid="{27F60B6A-AD95-4A31-B7BB-A255EBB1B59B}"/>
+    <hyperlink ref="A13" r:id="rId12" xr:uid="{D1701D65-C3E9-44B9-9432-6DE16CD43459}"/>
+    <hyperlink ref="A14" r:id="rId13" display="Deep Lattice Networks and Partial Monotonic Functions" xr:uid="{C40B8795-0355-46FD-85E9-F08955370F28}"/>
+    <hyperlink ref="A16" r:id="rId14" xr:uid="{958B5310-3407-4F42-BF4D-D61F37FFA816}"/>
+    <hyperlink ref="A17" r:id="rId15" xr:uid="{09E41EEB-2EC0-4EB6-88B7-8F6E25E15238}"/>
+    <hyperlink ref="A18" r:id="rId16" xr:uid="{72E3E7BC-7B2E-4618-A58A-149793960C7F}"/>
+    <hyperlink ref="A19" r:id="rId17" xr:uid="{20B83A96-428E-4479-A9D3-636F03504E2C}"/>
+    <hyperlink ref="A20" r:id="rId18" xr:uid="{D05401CB-7A16-46FE-82D1-13E9C9B73EBE}"/>
+    <hyperlink ref="A21" r:id="rId19" xr:uid="{9FD4428F-7748-4B69-9C49-BCD0EBA035C9}"/>
+    <hyperlink ref="A22" r:id="rId20" xr:uid="{FBDDE59E-EEC1-439C-A1C0-552D68A350ED}"/>
+    <hyperlink ref="A23" r:id="rId21" xr:uid="{DC3C4241-0BCD-4AA5-9599-E5C0FD1B0A67}"/>
+    <hyperlink ref="A24" r:id="rId22" xr:uid="{C50A4BC1-DC3A-4E06-AE5F-1FDA87C12F5E}"/>
+    <hyperlink ref="A25" r:id="rId23" xr:uid="{2F0F98AE-1E27-4C0D-9C25-E88E96D09296}"/>
+    <hyperlink ref="A26" r:id="rId24" xr:uid="{8FD0B6DE-815B-4968-BF82-F3A750F3FF0A}"/>
+    <hyperlink ref="A27" r:id="rId25" xr:uid="{4F8113ED-4F92-4A42-9BF6-8AE87E627AED}"/>
+    <hyperlink ref="A28" r:id="rId26" xr:uid="{042875D8-C34B-4E02-BDED-CE45E506DF4A}"/>
+    <hyperlink ref="A29" r:id="rId27" xr:uid="{02F2BFA7-7428-4B13-9C17-18BF77735185}"/>
+    <hyperlink ref="A30" r:id="rId28" xr:uid="{0B060E60-6089-4CFC-875F-4F2F9213E464}"/>
+    <hyperlink ref="L15" r:id="rId29" xr:uid="{5ED3FF45-3432-438F-B9AE-0455858A894A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId30"/>
-  <legacyDrawing r:id="rId31"/>
+  <drawing r:id="rId31"/>
+  <legacyDrawing r:id="rId32"/>
 </worksheet>
 </file>
</xml_diff>